<commit_message>
additional notes to task + made new ver. of chernovik.py
</commit_message>
<xml_diff>
--- a/6_Objective_Cell_Phones_Unlock/call_phones_unclock_task.xlsx
+++ b/6_Objective_Cell_Phones_Unlock/call_phones_unclock_task.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Разблокировка мобильных телефонов</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t xml:space="preserve">Раскладка точек блокировки:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">двигаться мы можем не только по уже отмеченной линии</t>
+  </si>
+  <si>
+    <t xml:space="preserve">у нас просто есть точки с цифрами</t>
+  </si>
+  <si>
+    <t xml:space="preserve">и между ними можно двигаться как угодно — но только к ближайшим соседям</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Типа 5-8 нельзя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">А 5-2 можно</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 — 8 будет просто через 2</t>
   </si>
   <si>
     <t xml:space="preserve">Ломаная линия разблокировки представляет собой последовательность цифр от 1 до 9, соответствующих точкам на этой</t>
@@ -86,9 +104,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -187,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +236,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,9 +266,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:colOff>750600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -259,7 +282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1774800"/>
-          <a:ext cx="4022280" cy="3903840"/>
+          <a:ext cx="4026960" cy="3903480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -279,13 +302,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -331,15 +354,39 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
+      <c r="G14" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
+      <c r="G15" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
+      <c r="G18" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G19" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
@@ -361,22 +408,22 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,7 +431,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -392,12 +439,12 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,7 +452,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -413,7 +460,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,7 +468,7 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -429,7 +476,7 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,12 +484,12 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,21 +497,21 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="0" t="n">
+      <c r="D57" s="7" t="n">
         <f aca="false">SQRT(POWER(1,2)+POWER(1,2))</f>
         <v>1.4142135623731</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="n">
+      <c r="A58" s="8" t="n">
         <f aca="false">1+1+1+1+1+1.41+1.41+1+1</f>
         <v>9.82</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="7" t="n">
         <f aca="false">7+D57+D57</f>
         <v>9.82842712474619</v>
       </c>

</xml_diff>